<commit_message>
Added Draw.io diagram of mathematical model
</commit_message>
<xml_diff>
--- a/Materials/LinkTemplate.xlsx
+++ b/Materials/LinkTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f1d977de6d9a3fe/Documents/The Arm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\wa-arm-structure\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="554" documentId="8_{8424CDF7-9186-4CB8-A812-B16A34F45486}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{98B46C7C-E2FB-47D8-8542-BEDE4B54BBBA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C1AE82-6469-45E6-AA96-71923F3AA090}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{732C66A2-6AAA-4FEE-96F2-21042206E23E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <definedName name="StructuralRodCrossSection">'Key figures'!$C$11</definedName>
     <definedName name="StructuralRodMaterial">'Key figures'!$C$10</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,6 +38,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1085,7 +1086,7 @@
                 <am3d:spPr>
                   <a:xfrm>
                     <a:off x="0" y="0"/>
-                    <a:ext cx="5348673" cy="3463372"/>
+                    <a:ext cx="5352483" cy="3463372"/>
                   </a:xfrm>
                   <a:prstGeom prst="rect">
                     <a:avLst/>
@@ -1166,8 +1167,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5515320" y="788588"/>
-              <a:ext cx="5348673" cy="3463372"/>
+              <a:off x="5513415" y="784778"/>
+              <a:ext cx="5352483" cy="3463372"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1597,7 +1598,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,7 +1750,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2947,7 +2948,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,20 +3707,23 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="27" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B4:K24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:K24">
     <sortCondition descending="1" ref="K4:K24"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1" xr:uid="{1A4E48FA-B6E8-4FF1-B20D-75D7B0339642}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>